<commit_message>
Deploying to gh-pages from  @ 40a8ac10c94fcd8ba614ff134d04a3f073c859be 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_1-4-2.xlsx
+++ b/assets/excel/2021_1-4-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring_2021\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E8ECE9-9BAE-41BA-9955-AFC3C0FF75E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7587C7A4-1772-4797-AD80-FF6AB80DD117}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{5B9D5FF7-0EDA-4F75-B44C-924FC8B4E454}"/>
   </bookViews>
@@ -256,6 +256,22 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -276,22 +292,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -833,30 +833,30 @@
       <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
-      <c r="R6" s="26"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="32"/>
     </row>
     <row r="7" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="7">
         <v>2005</v>
       </c>
@@ -907,76 +907,76 @@
       </c>
     </row>
     <row r="8" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24"/>
-      <c r="C8" s="27" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="28"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="33"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="34"/>
     </row>
     <row r="9" spans="2:18" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="33">
+      <c r="B9" s="26">
         <v>1</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="26">
         <v>2</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="26">
         <v>3</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="26">
         <v>4</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="26">
         <v>5</v>
       </c>
-      <c r="G9" s="33">
+      <c r="G9" s="26">
         <v>6</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="26">
         <v>7</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="26">
         <v>8</v>
       </c>
-      <c r="J9" s="33">
+      <c r="J9" s="26">
         <v>9</v>
       </c>
-      <c r="K9" s="33">
+      <c r="K9" s="26">
         <v>10</v>
       </c>
-      <c r="L9" s="33">
+      <c r="L9" s="26">
         <v>11</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="26">
         <v>12</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="26">
         <v>13</v>
       </c>
-      <c r="O9" s="34">
+      <c r="O9" s="27">
         <v>14</v>
       </c>
-      <c r="P9" s="33">
+      <c r="P9" s="26">
         <v>15</v>
       </c>
-      <c r="Q9" s="34">
+      <c r="Q9" s="27">
         <v>16</v>
       </c>
-      <c r="R9" s="34">
+      <c r="R9" s="27">
         <v>17</v>
       </c>
     </row>
@@ -1736,381 +1736,381 @@
         <v>1173</v>
       </c>
     </row>
-    <row r="24" spans="2:18" s="30" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B24" s="12" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B17</f>
         <v xml:space="preserve">  Türkei                    </v>
       </c>
-      <c r="C24" s="29">
+      <c r="C24" s="22">
         <v>2012</v>
       </c>
-      <c r="D24" s="29">
+      <c r="D24" s="22">
         <v>2046</v>
       </c>
-      <c r="E24" s="29">
+      <c r="E24" s="22">
         <v>1889</v>
       </c>
-      <c r="F24" s="29">
+      <c r="F24" s="22">
         <v>2159</v>
       </c>
-      <c r="G24" s="29">
+      <c r="G24" s="22">
         <v>2076</v>
       </c>
-      <c r="H24" s="29">
+      <c r="H24" s="22">
         <v>1817</v>
       </c>
-      <c r="I24" s="29">
+      <c r="I24" s="22">
         <v>1727</v>
       </c>
-      <c r="J24" s="29">
+      <c r="J24" s="22">
         <v>1743</v>
       </c>
-      <c r="K24" s="29">
+      <c r="K24" s="22">
         <v>1809</v>
       </c>
-      <c r="L24" s="29">
+      <c r="L24" s="22">
         <v>1821</v>
       </c>
-      <c r="M24" s="29">
+      <c r="M24" s="22">
         <v>1644</v>
       </c>
-      <c r="N24" s="29">
+      <c r="N24" s="22">
         <v>1926</v>
       </c>
-      <c r="O24" s="29">
+      <c r="O24" s="22">
         <v>1636</v>
       </c>
-      <c r="P24" s="29">
+      <c r="P24" s="22">
         <v>1901</v>
       </c>
-      <c r="Q24" s="29">
+      <c r="Q24" s="22">
         <v>1769</v>
       </c>
-      <c r="R24" s="29">
+      <c r="R24" s="22">
         <v>1395</v>
       </c>
     </row>
-    <row r="25" spans="2:18" s="30" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B25" s="12" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B18</f>
         <v xml:space="preserve">  Ukraine                   </v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="22">
         <v>441</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="22">
         <v>395</v>
       </c>
-      <c r="E25" s="29">
+      <c r="E25" s="22">
         <v>329</v>
       </c>
-      <c r="F25" s="29">
+      <c r="F25" s="22">
         <v>451</v>
       </c>
-      <c r="G25" s="29">
+      <c r="G25" s="22">
         <v>293</v>
       </c>
-      <c r="H25" s="29">
+      <c r="H25" s="22">
         <v>242</v>
       </c>
-      <c r="I25" s="29">
+      <c r="I25" s="22">
         <v>293</v>
       </c>
-      <c r="J25" s="29">
+      <c r="J25" s="22">
         <v>261</v>
       </c>
-      <c r="K25" s="29">
+      <c r="K25" s="22">
         <v>252</v>
       </c>
-      <c r="L25" s="29">
+      <c r="L25" s="22">
         <v>284</v>
       </c>
-      <c r="M25" s="29">
+      <c r="M25" s="22">
         <v>317</v>
       </c>
-      <c r="N25" s="29">
+      <c r="N25" s="22">
         <v>478</v>
       </c>
-      <c r="O25" s="29">
+      <c r="O25" s="22">
         <v>708</v>
       </c>
-      <c r="P25" s="29">
+      <c r="P25" s="22">
         <v>683</v>
       </c>
-      <c r="Q25" s="29">
+      <c r="Q25" s="22">
         <v>1070</v>
       </c>
-      <c r="R25" s="29">
+      <c r="R25" s="22">
         <v>752</v>
       </c>
     </row>
-    <row r="26" spans="2:18" s="30" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B26" s="12" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B19</f>
         <v xml:space="preserve">  Ungarn                    </v>
       </c>
-      <c r="C26" s="29">
+      <c r="C26" s="22">
         <v>1435</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="22">
         <v>1719</v>
       </c>
-      <c r="E26" s="29">
+      <c r="E26" s="22">
         <v>2058</v>
       </c>
-      <c r="F26" s="29">
+      <c r="F26" s="22">
         <v>2415</v>
       </c>
-      <c r="G26" s="29">
+      <c r="G26" s="22">
         <v>2632</v>
       </c>
-      <c r="H26" s="29">
+      <c r="H26" s="22">
         <v>2054</v>
       </c>
-      <c r="I26" s="29">
+      <c r="I26" s="22">
         <v>2534</v>
       </c>
-      <c r="J26" s="29">
+      <c r="J26" s="22">
         <v>2651</v>
       </c>
-      <c r="K26" s="29">
+      <c r="K26" s="22">
         <v>3419</v>
       </c>
-      <c r="L26" s="29">
+      <c r="L26" s="22">
         <v>3489</v>
       </c>
-      <c r="M26" s="29">
+      <c r="M26" s="22">
         <v>2997</v>
       </c>
-      <c r="N26" s="29">
+      <c r="N26" s="22">
         <v>3035</v>
       </c>
-      <c r="O26" s="29">
+      <c r="O26" s="22">
         <v>2765</v>
       </c>
-      <c r="P26" s="29">
+      <c r="P26" s="22">
         <v>2578</v>
       </c>
-      <c r="Q26" s="29">
+      <c r="Q26" s="22">
         <v>2332</v>
       </c>
-      <c r="R26" s="29">
+      <c r="R26" s="22">
         <v>2020</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="30" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:18" s="23" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B27" s="12" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B20</f>
         <v xml:space="preserve">  Vereinigtes Königreich, Nordirland</v>
       </c>
-      <c r="C27" s="29">
+      <c r="C27" s="22">
         <v>1329</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="22">
         <v>1428</v>
       </c>
-      <c r="E27" s="29">
+      <c r="E27" s="22">
         <v>1242</v>
       </c>
-      <c r="F27" s="29">
+      <c r="F27" s="22">
         <v>1434</v>
       </c>
-      <c r="G27" s="29">
+      <c r="G27" s="22">
         <v>1435</v>
       </c>
-      <c r="H27" s="29">
+      <c r="H27" s="22">
         <v>1176</v>
       </c>
-      <c r="I27" s="29">
+      <c r="I27" s="22">
         <v>1276</v>
       </c>
-      <c r="J27" s="29">
+      <c r="J27" s="22">
         <v>1177</v>
       </c>
-      <c r="K27" s="29">
+      <c r="K27" s="22">
         <v>1227</v>
       </c>
-      <c r="L27" s="29">
+      <c r="L27" s="22">
         <v>1531</v>
       </c>
-      <c r="M27" s="29">
+      <c r="M27" s="22">
         <v>1497</v>
       </c>
-      <c r="N27" s="29">
+      <c r="N27" s="22">
         <v>1339</v>
       </c>
-      <c r="O27" s="29">
+      <c r="O27" s="22">
         <v>1090</v>
       </c>
-      <c r="P27" s="29">
+      <c r="P27" s="22">
         <v>1193</v>
       </c>
-      <c r="Q27" s="29">
+      <c r="Q27" s="22">
         <v>1200</v>
       </c>
-      <c r="R27" s="29">
+      <c r="R27" s="22">
         <v>887</v>
       </c>
     </row>
-    <row r="28" spans="2:18" s="32" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:18" s="25" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B28" s="9" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B21</f>
         <v xml:space="preserve"> EU Staaten                 </v>
       </c>
-      <c r="C28" s="31">
+      <c r="C28" s="24">
         <v>35054</v>
       </c>
-      <c r="D28" s="31">
+      <c r="D28" s="24">
         <v>37538</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="24">
         <v>40122</v>
       </c>
-      <c r="F28" s="31">
+      <c r="F28" s="24">
         <v>44373</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="24">
         <v>44947</v>
       </c>
-      <c r="H28" s="31">
+      <c r="H28" s="24">
         <v>41807</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="24">
         <v>47208</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="24">
         <v>50761</v>
       </c>
-      <c r="K28" s="31">
+      <c r="K28" s="24">
         <v>55590</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L28" s="24">
         <v>61810</v>
       </c>
-      <c r="M28" s="31">
+      <c r="M28" s="24">
         <v>58568</v>
       </c>
-      <c r="N28" s="31">
+      <c r="N28" s="24">
         <v>68721</v>
       </c>
-      <c r="O28" s="31">
+      <c r="O28" s="24">
         <v>62569</v>
       </c>
-      <c r="P28" s="31">
+      <c r="P28" s="24">
         <v>69033</v>
       </c>
-      <c r="Q28" s="31">
+      <c r="Q28" s="24">
         <v>71647</v>
       </c>
-      <c r="R28" s="31">
+      <c r="R28" s="24">
         <v>55071</v>
       </c>
     </row>
-    <row r="29" spans="2:18" s="32" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:18" s="25" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B29" s="9" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B22</f>
         <v xml:space="preserve">Afrika insgesamt            </v>
       </c>
-      <c r="C29" s="31">
+      <c r="C29" s="24">
         <v>1545</v>
       </c>
-      <c r="D29" s="31">
+      <c r="D29" s="24">
         <v>1512</v>
       </c>
-      <c r="E29" s="31">
+      <c r="E29" s="24">
         <v>1367</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="24">
         <v>1598</v>
       </c>
-      <c r="G29" s="31">
+      <c r="G29" s="24">
         <v>1348</v>
       </c>
-      <c r="H29" s="31">
+      <c r="H29" s="24">
         <v>1208</v>
       </c>
-      <c r="I29" s="31">
+      <c r="I29" s="24">
         <v>1259</v>
       </c>
-      <c r="J29" s="31">
+      <c r="J29" s="24">
         <v>1257</v>
       </c>
-      <c r="K29" s="31">
+      <c r="K29" s="24">
         <v>1355</v>
       </c>
-      <c r="L29" s="31">
+      <c r="L29" s="24">
         <v>2023</v>
       </c>
-      <c r="M29" s="31">
+      <c r="M29" s="24">
         <v>2438</v>
       </c>
-      <c r="N29" s="31">
+      <c r="N29" s="24">
         <v>6689</v>
       </c>
-      <c r="O29" s="31">
+      <c r="O29" s="24">
         <v>4200</v>
       </c>
-      <c r="P29" s="31">
+      <c r="P29" s="24">
         <v>2701</v>
       </c>
-      <c r="Q29" s="31">
+      <c r="Q29" s="24">
         <v>2560</v>
       </c>
-      <c r="R29" s="31">
+      <c r="R29" s="24">
         <v>2013</v>
       </c>
     </row>
-    <row r="30" spans="2:18" s="32" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:18" s="25" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B30" s="9" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B23</f>
         <v xml:space="preserve">Amerika insgesamt           </v>
       </c>
-      <c r="C30" s="31">
+      <c r="C30" s="24">
         <v>3678</v>
       </c>
-      <c r="D30" s="31">
+      <c r="D30" s="24">
         <v>3627</v>
       </c>
-      <c r="E30" s="31">
+      <c r="E30" s="24">
         <v>4031</v>
       </c>
-      <c r="F30" s="31">
+      <c r="F30" s="24">
         <v>5228</v>
       </c>
-      <c r="G30" s="31">
+      <c r="G30" s="24">
         <v>4375</v>
       </c>
-      <c r="H30" s="31">
+      <c r="H30" s="24">
         <v>4047</v>
       </c>
-      <c r="I30" s="31">
+      <c r="I30" s="24">
         <v>4034</v>
       </c>
-      <c r="J30" s="31">
+      <c r="J30" s="24">
         <v>3832</v>
       </c>
-      <c r="K30" s="31">
+      <c r="K30" s="24">
         <v>3847</v>
       </c>
-      <c r="L30" s="31">
+      <c r="L30" s="24">
         <v>4067</v>
       </c>
-      <c r="M30" s="31">
+      <c r="M30" s="24">
         <v>3859</v>
       </c>
-      <c r="N30" s="31">
+      <c r="N30" s="24">
         <v>4286</v>
       </c>
-      <c r="O30" s="31">
+      <c r="O30" s="24">
         <v>3611</v>
       </c>
-      <c r="P30" s="31">
+      <c r="P30" s="24">
         <v>3577</v>
       </c>
-      <c r="Q30" s="31">
+      <c r="Q30" s="24">
         <v>3820</v>
       </c>
-      <c r="R30" s="31">
+      <c r="R30" s="24">
         <v>2624</v>
       </c>
     </row>
@@ -2276,57 +2276,57 @@
         <v>1309</v>
       </c>
     </row>
-    <row r="34" spans="2:18" s="32" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:18" s="25" customFormat="1" ht="8.25" x14ac:dyDescent="0.15">
       <c r="B34" s="9" t="str">
         <f>'[1]2020_1-4-2_Rohdaten'!B27</f>
         <v xml:space="preserve">Australien und Ozeanien     </v>
       </c>
-      <c r="C34" s="31">
+      <c r="C34" s="24">
         <v>396</v>
       </c>
-      <c r="D34" s="31">
+      <c r="D34" s="24">
         <v>413</v>
       </c>
-      <c r="E34" s="31">
+      <c r="E34" s="24">
         <v>502</v>
       </c>
-      <c r="F34" s="31">
+      <c r="F34" s="24">
         <v>608</v>
       </c>
-      <c r="G34" s="31">
+      <c r="G34" s="24">
         <v>562</v>
       </c>
-      <c r="H34" s="31">
+      <c r="H34" s="24">
         <v>547</v>
       </c>
-      <c r="I34" s="31">
+      <c r="I34" s="24">
         <v>535</v>
       </c>
-      <c r="J34" s="31">
+      <c r="J34" s="24">
         <v>500</v>
       </c>
-      <c r="K34" s="31">
+      <c r="K34" s="24">
         <v>554</v>
       </c>
-      <c r="L34" s="31">
+      <c r="L34" s="24">
         <v>572</v>
       </c>
-      <c r="M34" s="31">
+      <c r="M34" s="24">
         <v>531</v>
       </c>
-      <c r="N34" s="31">
+      <c r="N34" s="24">
         <v>593</v>
       </c>
-      <c r="O34" s="31">
+      <c r="O34" s="24">
         <v>566</v>
       </c>
-      <c r="P34" s="31">
+      <c r="P34" s="24">
         <v>524</v>
       </c>
-      <c r="Q34" s="31">
+      <c r="Q34" s="24">
         <v>497</v>
       </c>
-      <c r="R34" s="31">
+      <c r="R34" s="24">
         <v>287</v>
       </c>
     </row>

</xml_diff>